<commit_message>
Changed hasFile to hasPart
</commit_message>
<xml_diff>
--- a/cooee-attachments/ro-crate-metadata.xlsx
+++ b/cooee-attachments/ro-crate-metadata.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -58,7 +58,7 @@
     <t>hasPart</t>
   </si>
   <si>
-    <t>["3-COOEE-4.doc", "COOEE contents.XLS", "COOEE.XLS", "COOEE_contents.xlsx", "data/", "data"]</t>
+    <t>["3-COOEE-4.doc", "COOEE contents.XLS", "COOEE.XLS", "COOEE_contents.xlsx", "data/", "data/", "COOEE_contents_original.xlsx", {"@id":"data"}]</t>
   </si>
   <si>
     <t>license</t>
@@ -82,15 +82,12 @@
     <t>hasFile</t>
   </si>
   <si>
-    <t>["3-COOEE-4.doc", "COOEE contents.XLS", "COOEE.XLS", "COOEE_contents.xlsx", "COOEE_contents_original.xlsx"]</t>
+    <t>[]</t>
   </si>
   <si>
     <t>data/</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>["data/1-001-plain.txt", "data/1-001.txt", "data/1-002-plain.txt", "data/1-002.txt", "data/1-003-plain.txt", "data/1-003.txt", "data/1-004-plain.txt", "data/1-004.txt", "data/1-005-plain.txt", "data/1-005.txt", "data/1-006-plain.txt", "data/1-006.txt", "data/1-007-plain.txt", "data/1-007.txt", "data/1-008-plain.txt", "data/1-008.txt", "data/1-009-plain.txt", "data/1-009.txt", "data/1-010-plain.txt", "data/1-010.txt", "data/1-011-plain.txt", "data/1-011.txt", "data/1-012-plain.txt", "data/1-012.txt", "data/1-013-plain.txt", "data/1-013.txt", "data/1-014-plain.txt", "data/1-014.txt", "data/1-015-plain.txt", "data/1-015.txt", "data/1-016-plain.txt", "data/1-016.txt", "data/1-017-plain.txt", "data/1-017.txt", "data/1-018-plain.txt", "data/1-018.txt", "data/1-019-plain.txt", "data/1-019.txt", "data/1-020-plain.txt", "data/1-020.txt", "data/1-021-plain.txt", "data/1-021.txt", "data/1-022-plain.txt", "data/1-022.txt", "data/1-023-plain.txt", "data/1-023.txt", "data/1-024-plain.txt", "data/1-024.txt", "data/1-025-plain.txt", "data/1-025.txt", "data/1-026-plain.txt", "data/1-026.txt", "data/1-027-plain.txt", "data/1-027.txt", "data/1-028-plain.txt", "data/1-028.txt", "data/1-029-plain.txt", "data/1-029.txt", "data/1-030-plain.txt", "data/1-030.txt", "data/1-031-plain.txt", "data/1-031.txt", "data/1-032-plain.txt", "data/1-032.txt", "data/1-033-plain.txt", "data/1-033.txt", "data/1-034-plain.txt", "data/1-034.txt", "data/1-035-plain.txt", "data/1-035.txt", "data/1-037-plain.txt", "data/1-037.txt", "data/1-038-plain.txt", "data/1-038.txt", "data/1-039-plain.txt", "data/1-039.txt", "data/1-040-plain.txt", "data/1-040.txt", "data/1-041-plain.txt", "data/1-041.txt", "data/1-043-plain.txt", "data/1-043.txt", "data/1-044-plain.txt", "data/1-044.txt", "data/1-045-plain.txt", "data/1-045.txt", "data/1-046-plain.txt", "data/1-046.txt", "data/1-047-plain.txt", "data/1-047.txt", "data/1-048-plain.txt", "data/1-048.txt", "data/1-049-plain.txt", "data/1-049.txt", "data/1-050-plain.txt", "data/1-050.txt", "data/1-051-plain.txt", "data/1-051.txt", "data/1-052-plain.txt", "data/1-052.txt", "data/1-053-plain.txt", "data/1-053.txt", "data/1-054-plain.txt", "data/1-054.txt", "data/1-055-plain.txt", "data/1-055.txt", "data/1-058-plain.txt", "data/1-058.txt", "data/1-059-plain.txt", "data/1-059.txt", "data/1-060-plain.txt", "data/1-060.txt", "data/1-061-plain.txt", "data/1-061.txt", "data/1-062-plain.txt", "data/1-062.txt", "data/1-063-plain.txt", "data/1-063.txt", "data/1-064-plain.txt", "data/1-064.txt", "data/1-065-plain.txt", "data/1-065.txt", "data/1-066-plain.txt", "data/1-066.txt", "data/1-067-plain.txt", "data/1-067.txt", "data/1-068-plain.txt", "data/1-068.txt", "data/1-069-plain.txt", "data/1-069.txt", "data/1-070-plain.txt", "data/1-070.txt", "data/1-071-plain.txt", "data/1-071.txt", "data/1-072-plain.txt", "data/1-072.txt", "data/1-073-plain.txt", "data/1-073.txt", "data/1-074-plain.txt", "data/1-074.txt", "data/1-075-plain.txt", "data/1-075.txt", "data/1-076-plain.txt", "data/1-076.txt", "data/1-077-plain.txt", "data/1-077.txt", "data/1-078-plain.txt", "data/1-078.txt", "data/1-079-plain.txt", "data/1-079.txt", "data/1-080-plain.txt", "data/1-080.txt", "data/1-081-plain.txt", "data/1-081.txt", "data/1-082-plain.txt", "data/1-082.txt", "data/1-083-plain.txt", "data/1-083.txt", "data/1-084-plain.txt", "data/1-084.txt", "data/1-085-plain.txt", "data/1-085.txt", "data/1-086-plain.txt", "data/1-086.txt", "data/1-087-plain.txt", "data/1-087.txt", "data/1-088-plain.txt", "data/1-088.txt", "data/1-089-plain.txt", "data/1-089.txt", "data/1-091-plain.txt", "data/1-091.txt", "data/1-092-plain.txt", "data/1-092.txt", "data/1-093-plain.txt", "data/1-093.txt", "data/1-094-plain.txt", "data/1-094.txt", "data/1-095-plain.txt", "data/1-095.txt", "data/1-096-plain.txt", "data/1-096.txt", "data/1-097-plain.txt", "data/1-097.txt", "data/1-098-plain.txt", "data/1-098.txt", "data/1-099-plain.txt", "data/1-099.txt", "data/1-100-plain.txt", "data/1-100.txt", "data/1-101-plain.txt", "data/1-101.txt", "data/1-102-plain.txt", "data/1-102.txt", "data/1-103-plain.txt", "data/1-103.txt", "data/1-104-plain.txt", "data/1-104.txt", "data/1-105-plain.txt", "data/1-105.txt", "data/1-106-plain.txt", "data/1-106.txt", "data/1-107-plain.txt", "data/1-107.txt", "data/1-108-plain.txt", "data/1-108.txt", "data/1-109-plain.txt", "data/1-109.txt", "data/1-110-plain.txt", "data/1-110.txt", "data/1-111-plain.txt", "data/1-111.txt", "data/1-112-plain.txt", "data/1-112.txt", "data/1-113-plain.txt", "data/1-113.txt", "data/1-114-plain.txt", "data/1-114.txt", "data/1-115-plain.txt", "data/1-115.txt", "data/1-116-plain.txt", "data/1-116.txt", "data/1-117-plain.txt", "data/1-117.txt", "data/1-118-plain.txt", "data/1-118.txt", "data/1-119-plain.txt", "data/1-119.txt", "data/1-120-plain.txt", "data/1-120.txt", "data/1-121-plain.txt", "data/1-121.txt", "data/1-122-plain.txt", "data/1-122.txt", "data/1-124-plain.txt", "data/1-124.txt", "data/1-125-plain.txt", "data/1-125.txt", "data/1-126-plain.txt", "data/1-126.txt", "data/1-127-plain.txt", "data/1-127.txt", "data/1-128-plain.txt", "data/1-128.txt", "data/1-129-plain.txt", "data/1-129.txt", "data/1-130-plain.txt", "data/1-130.txt", "data/1-131-plain.txt", "data/1-131.txt", "data/1-132-plain.txt", "data/1-132.txt", "data/1-133-plain.txt", "data/1-133.txt", "data/1-134-plain.txt", "data/1-134.txt", "data/1-135-plain.txt", "data/1-135.txt", "data/1-136-plain.txt", "data/1-136.txt", "data/1-137-plain.txt", "data/1-137.txt", "data/1-138-plain.txt", "data/1-138.txt", "data/1-139-plain.txt", "data/1-139.txt", "data/1-140-plain.txt", "data/1-140.txt", "data/1-141-plain.txt", "data/1-141.txt", "data/1-142-plain.txt", "data/1-142.txt", "data/1-143-plain.txt", "data/1-143.txt", "data/1-144-plain.txt", "data/1-144.txt", "data/1-145-plain.txt", "data/1-145.txt", "data/1-146-plain.txt", "data/1-146.txt", "data/1-147-plain.txt", "data/1-147.txt", "data/1-148-plain.txt", "data/1-148.txt", "data/1-149-plain.txt", "data/1-149.txt", "data/1-150-plain.txt", "data/1-150.txt", "data/1-151-plain.txt", "data/1-151.txt", "data/1-152-plain.txt", "data/1-152.txt", "data/1-153-plain.txt", "data/1-153.txt", "data/1-154-plain.txt", "data/1-154.txt", "data/1-155-plain.txt", "data/1-155.txt", "data/1-156-plain.txt", "data/1-156.txt", "data/1-157-plain.txt", "data/1-157.txt", "data/1-158-plain.txt", "data/1-158.txt", "data/1-159-plain.txt", "data/1-159.txt", "data/1-160-plain.txt", "data/1-160.txt", "data/1-161-plain.txt", "data/1-161.txt", "data/1-162-plain.txt", "data/1-162.txt", "data/1-163-plain.txt", "data/1-163.txt", "data/1-164-plain.txt", "data/1-164.txt", "data/1-165-plain.txt", "data/1-165.txt", "data/1-166-plain.txt", "data/1-166.txt", "data/1-167-plain.txt", "data/1-167.txt", "data/1-168-plain.txt", "data/1-168.txt", "data/1-169-plain.txt", "data/1-169.txt", "data/1-170-plain.txt", "data/1-170.txt", "data/1-171-plain.txt", "data/1-171.txt", "data/1-172-plain.txt", "data/1-172.txt", "data/1-173-plain.txt", "data/1-173.txt", "data/1-174-plain.txt", "data/1-174.txt", "data/1-175-plain.txt", "data/1-175.txt", "data/1-176-plain.txt", "data/1-176.txt", "data/1-177-plain.txt", "data/1-177.txt", "data/1-178-plain.txt", "data/1-178.txt", "data/1-179-plain.txt", "data/1-179.txt", "data/1-180-plain.txt", "data/1-180.txt", "data/1-181-plain.txt", "data/1-181.txt", "data/1-182-plain.txt", "data/1-182.txt", "data/1-183-plain.txt", "data/1-183.txt", "data/1-184-plain.txt", "data/1-184.txt", "data/1-185-plain.txt", "data/1-185.txt", "data/1-186-plain.txt", "data/1-186.txt", "data/1-187-plain.txt", "data/1-187.txt", "data/1-188-plain.txt", "data/1-188.txt", "data/1-189-plain.txt", "data/1-189.txt", "data/1-190-plain.txt", "data/1-190.txt", "data/1-191-plain.txt", "data/1-191.txt", "data/1-192-plain.txt", "data/1-192.txt", "data/1-193-plain.txt", "data/1-193.txt", "data/1-194-plain.txt", "data/1-194.txt", "data/1-195-plain.txt", "data/1-195.txt", "data/1-196-plain.txt", "data/1-196.txt", "data/1-197-plain.txt", "data/1-197.txt", "data/1-198-plain.txt", "data/1-198.txt", "data/1-199-plain.txt", "data/1-199.txt", "data/1-200-plain.txt", "data/1-200.txt", "data/1-201-plain.txt", "data/1-201.txt", "data/1-202-plain.txt", "data/1-202.txt", "data/1-203-plain.txt", "data/1-203.txt", "data/1-204-plain.txt", "data/1-204.txt", "data/1-205-plain.txt", "data/1-205.txt", "data/1-206-plain.txt", "data/1-206.txt", "data/1-207-plain.txt", "data/1-207.txt", "data/1-208-plain.txt", "data/1-208.txt", "data/1-209-plain.txt", "data/1-209.txt", "data/1-210-plain.txt", "data/1-210.txt", "data/1-211-plain.txt", "data/1-211.txt", "data/1-212-plain.txt", "data/1-212.txt", "data/1-213-plain.txt", "data/1-213.txt", "data/1-214-plain.txt", "data/1-214.txt", "data/1-215-plain.txt", "data/1-215.txt", "data/1-216-plain.txt", "data/1-216.txt", "data/1-217-plain.txt", "data/1-217.txt", "data/1-218-plain.txt", "data/1-218.txt", "data/1-219-plain.txt", "data/1-219.txt", "data/1-220-plain.txt", "data/1-220.txt", "data/1-221-plain.txt", "data/1-221.txt", "data/1-222-plain.txt", "data/1-222.txt", "data/1-223-plain.txt", "data/1-223.txt", "data/1-224-plain.txt", "data/1-224.txt", "data/1-225-plain.txt", "data/1-225.txt", "data/1-226-plain.txt", "data/1-226.txt", "data/1-227-plain.txt", "data/1-227.txt", "data/1-228-plain.txt", "data/1-228.txt", "data/1-229-plain.txt", "data/1-229.txt", "data/1-230-plain.txt", "data/1-230.txt", "data/1-231-plain.txt", "data/1-231.txt", "data/1-232-plain.txt", "data/1-232.txt", "data/1-233-plain.txt", "data/1-233.txt", "data/1-234-plain.txt", "data/1-234.txt", "data/1-235-plain.txt", "data/1-235.txt", "data/1-236-plain.txt", "data/1-236.txt", "data/1-237-plain.txt", "data/1-237.txt", "data/1-238-plain.txt", "data/1-238.txt", "data/1-239-plain.txt", "data/1-239.txt", "data/1-240-plain.txt", "data/1-240.txt", "data/1-241-plain.txt", "data/1-241.txt", "data/1-242-plain.txt", "data/1-242.txt", "data/1-243-plain.txt", "data/1-243.txt", "data/1-244-plain.txt", "data/1-244.txt", "data/1-245-plain.txt", "data/1-245.txt", "data/1-246-plain.txt", "data/1-246.txt", "data/1-247-plain.txt", "data/1-247.txt", "data/1-248-plain.txt", "data/1-248.txt", "data/1-249-plain.txt", "data/1-249.txt", "data/1-250-plain.txt", "data/1-250.txt", "data/1-251-plain.txt", "data/1-251.txt", "data/1-252-plain.txt", "data/1-252.txt", "data/1-253-plain.txt", "data/1-253.txt", "data/1-254-plain.txt", "data/1-254.txt", "data/1-255-plain.txt", "data/1-255.txt", "data/1-256-plain.txt", "data/1-256.txt", "data/1-258-plain.txt", "data/1-258.txt", "data/1-259-plain.txt", "data/1-259.txt", "data/1-260-plain.txt", "data/1-260.txt", "data/1-261-plain.txt", "data/1-261.txt", "data/1-262-plain.txt", "data/1-262.txt", "data/1-263-plain.txt", "data/1-263.txt", "data/1-264-plain.txt", "data/1-264.txt", "data/1-265-plain.txt", "data/1-265.txt", "data/1-266-plain.txt", "data/1-266.txt", "data/1-267-plain.txt", "data/1-267.txt", "data/1-268-plain.txt", "data/1-268.txt", "data/1-269-plain.txt", "data/1-269.txt", "data/1-270-plain.txt", "data/1-270.txt", "data/1-271-plain.txt", "data/1-271.txt", "data/1-272-plain.txt", "data/1-272.txt", "data/2-001-plain.txt", "data/2-001.txt", "data/2-003-plain.txt", "data/2-003.txt", "data/2-004-plain.txt", "data/2-004.txt", "data/2-005-plain.txt", "data/2-005.txt", "data/2-006-plain.txt", "data/2-006.txt", "data/2-007-plain.txt", "data/2-007.txt", "data/2-008-plain.txt", "data/2-008.txt", "data/2-009-plain.txt", "data/2-009.txt", "data/2-010-plain.txt", "data/2-010.txt", "data/2-011-plain.txt", "data/2-011.txt", "data/2-012-plain.txt", "data/2-012.txt", "data/2-013-plain.txt", "data/2-013.txt", "data/2-014-plain.txt", "data/2-014.txt", "data/2-015-plain.txt", "data/2-015.txt", "data/2-016-plain.txt", "data/2-016.txt", "data/2-017-plain.txt", "data/2-017.txt", "data/2-018-plain.txt", "data/2-018.txt", "data/2-019-plain.txt", "data/2-019.txt", "data/2-020-plain.txt", "data/2-020.txt", "data/2-021-plain.txt", "data/2-021.txt", "data/2-022-plain.txt", "data/2-022.txt", "data/2-023-plain.txt", "data/2-023.txt", "data/2-024-plain.txt", "data/2-024.txt", "data/2-025-plain.txt", "data/2-025.txt", "data/2-026-plain.txt", "data/2-026.txt", "data/2-027-plain.txt", "data/2-027.txt", "data/2-028-plain.txt", "data/2-028.txt", "data/2-029-plain.txt", "data/2-029.txt", "data/2-030-plain.txt", "data/2-030.txt", "data/2-031-plain.txt", "data/2-031.txt", "data/2-032-plain.txt", "data/2-032.txt", "data/2-033-plain.txt", "data/2-033.txt", "data/2-034-plain.txt", "data/2-034.txt", "data/2-035-plain.txt", "data/2-035.txt", "data/2-036-plain.txt", "data/2-036.txt", "data/2-037-plain.txt", "data/2-037.txt", "data/2-038-plain.txt", "data/2-038.txt", "data/2-039-plain.txt", "data/2-039.txt", "data/2-040-plain.txt", "data/2-040.txt", "data/2-041-plain.txt", "data/2-041.txt", "data/2-042-plain.txt", "data/2-042.txt", "data/2-043-plain.txt", "data/2-043.txt", "data/2-044-plain.txt", "data/2-044.txt", "data/2-045-plain.txt", "data/2-045.txt", "data/2-046-plain.txt", "data/2-046.txt", "data/2-047-plain.txt", "data/2-047.txt", "data/2-048-plain.txt", "data/2-048.txt", "data/2-049-plain.txt", "data/2-049.txt", "data/2-050-plain.txt", "data/2-050.txt", "data/2-051-plain.txt", "data/2-051.txt", "data/2-052-plain.txt", "data/2-052.txt", "data/2-053-plain.txt", "data/2-053.txt", "data/2-054-plain.txt", "data/2-054.txt", "data/2-055-plain.txt", "data/2-055.txt", "data/2-056-plain.txt", "data/2-056.txt", "data/2-057-plain.txt", "data/2-057.txt", "data/2-058-plain.txt", "data/2-058.txt", "data/2-059-plain.txt", "data/2-059.txt", "data/2-060-plain.txt", "data/2-060.txt", "data/2-061-plain.txt", "data/2-061.txt", "data/2-062-plain.txt", "data/2-062.txt", "data/2-063-plain.txt", "data/2-063.txt", "data/2-064-plain.txt", "data/2-064.txt", "data/2-065-plain.txt", "data/2-065.txt", "data/2-066-plain.txt", "data/2-066.txt", "data/2-067-plain.txt", "data/2-067.txt", "data/2-068-plain.txt", "data/2-068.txt", "data/2-069-plain.txt", "data/2-069.txt", "data/2-070-plain.txt", "data/2-070.txt", "data/2-071-plain.txt", "data/2-071.txt", "data/2-072-plain.txt", "data/2-072.txt", "data/2-073-plain.txt", "data/2-073.txt", "data/2-074-plain.txt", "data/2-074.txt", "data/2-075-plain.txt", "data/2-075.txt", "data/2-076-plain.txt", "data/2-076.txt", "data/2-077-plain.txt", "data/2-077.txt", "data/2-079-plain.txt", "data/2-079.txt", "data/2-080-plain.txt", "data/2-080.txt", "data/2-081-plain.txt", "data/2-081.txt", "data/2-082-plain.txt", "data/2-082.txt", "data/2-083-plain.txt", "data/2-083.txt", "data/2-084-plain.txt", "data/2-084.txt", "data/2-085-plain.txt", "data/2-085.txt", "data/2-086-plain.txt", "data/2-086.txt", "data/2-087-plain.txt", "data/2-087.txt", "data/2-088-plain.txt", "data/2-088.txt", "data/2-089-plain.txt", "data/2-089.txt", "data/2-090-plain.txt", "data/2-090.txt", "data/2-091-plain.txt", "data/2-091.txt", "data/2-092-plain.txt", "data/2-092.txt", "data/2-093-plain.txt", "data/2-093.txt", "data/2-094-plain.txt", "data/2-094.txt", "data/2-095-plain.txt", "data/2-095.txt", "data/2-096-plain.txt", "data/2-096.txt", "data/2-097-plain.txt", "data/2-097.txt", "data/2-098-plain.txt", "data/2-098.txt", "data/2-099-plain.txt", "data/2-099.txt", "data/2-100-plain.txt", "data/2-100.txt", "data/2-101-plain.txt", "data/2-101.txt", "data/2-102-plain.txt", "data/2-102.txt", "data/2-103-plain.txt", "data/2-103.txt", "data/2-104-plain.txt", "data/2-104.txt", "data/2-105-plain.txt", "data/2-105.txt", "data/2-106-plain.txt", "data/2-106.txt", "data/2-107-plain.txt", "data/2-107.txt", "data/2-108-plain.txt", "data/2-108.txt", "data/2-109-plain.txt", "data/2-109.txt", "data/2-110-plain.txt", "data/2-110.txt", "data/2-111-plain.txt", "data/2-111.txt", "data/2-112-plain.txt", "data/2-112.txt", "data/2-113-plain.txt", "data/2-113.txt", "data/2-114-plain.txt", "data/2-114.txt", "data/2-115-plain.txt", "data/2-115.txt", "data/2-116-plain.txt", "data/2-116.txt", "data/2-117-plain.txt", "data/2-117.txt", "data/2-118-plain.txt", "data/2-118.txt", "data/2-119-plain.txt", "data/2-119.txt", "data/2-120-plain.txt", "data/2-120.txt", "data/2-121-plain.txt", "data/2-121.txt", "data/2-122-plain.txt", "data/2-122.txt", "data/2-123-plain.txt", "data/2-123.txt", "data/2-124-plain.txt", "data/2-124.txt", "data/2-125-plain.txt", "data/2-125.txt", "data/2-126-plain.txt", "data/2-126.txt", "data/2-127-plain.txt", "data/2-127.txt", "data/2-128-plain.txt", "data/2-128.txt", "data/2-129-plain.txt", "data/2-129.txt", "data/2-130-plain.txt", "data/2-130.txt", "data/2-131-plain.txt", "data/2-131.txt", "data/2-132-plain.txt", "data/2-132.txt", "data/2-133-plain.txt", "data/2-133.txt", "data/2-134-plain.txt", "data/2-134.txt", "data/2-135-plain.txt", "data/2-135.txt", "data/2-136-plain.txt", "data/2-136.txt", "data/2-137-plain.txt", "data/2-137.txt", "data/2-138-plain.txt", "data/2-138.txt", "data/2-139-plain.txt", "data/2-139.txt", "data/2-140-plain.txt", "data/2-140.txt", "data/2-141-plain.txt", "data/2-141.txt", "data/2-142-plain.txt", "data/2-142.txt", "data/2-143-plain.txt", "data/2-143.txt", "data/2-144-plain.txt", "data/2-144.txt", "data/2-145-plain.txt", "data/2-145.txt", "data/2-146-plain.txt", "data/2-146.txt", "data/2-147-plain.txt", "data/2-147.txt", "data/2-148-plain.txt", "data/2-148.txt", "data/2-149-plain.txt", "data/2-149.txt", "data/2-150-plain.txt", "data/2-150.txt", "data/2-151-plain.txt", "data/2-151.txt", "data/2-152-plain.txt", "data/2-152.txt", "data/2-153-plain.txt", "data/2-153.txt", "data/2-154-plain.txt", "data/2-154.txt", "data/2-155-plain.txt", "data/2-155.txt", "data/2-156-plain.txt", "data/2-156.txt", "data/2-157-plain.txt", "data/2-157.txt", "data/2-158-plain.txt", "data/2-158.txt", "data/2-159-plain.txt", "data/2-159.txt", "data/2-160-plain.txt", "data/2-160.txt", "data/2-161-plain.txt", "data/2-161.txt", "data/2-162-plain.txt", "data/2-162.txt", "data/2-163-plain.txt", "data/2-163.txt", "data/2-164-plain.txt", "data/2-164.txt", "data/2-165-plain.txt", "data/2-165.txt", "data/2-166-plain.txt", "data/2-166.txt", "data/2-167-plain.txt", "data/2-167.txt", "data/2-168-plain.txt", "data/2-168.txt", "data/2-169-plain.txt", "data/2-169.txt", "data/2-170-plain.txt", "data/2-170.txt", "data/2-171-plain.txt", "data/2-171.txt", "data/2-172-plain.txt", "data/2-172.txt", "data/2-173-plain.txt", "data/2-173.txt", "data/2-174-plain.txt", "data/2-174.txt", "data/2-175-plain.txt", "data/2-175.txt", "data/2-176-plain.txt", "data/2-176.txt", "data/2-177-plain.txt", "data/2-177.txt", "data/2-178-plain.txt", "data/2-178.txt", "data/2-179-plain.txt", "data/2-179.txt", "data/2-180-plain.txt", "data/2-180.txt", "data/2-181-plain.txt", "data/2-181.txt", "data/2-182-plain.txt", "data/2-182.txt", "data/2-183-plain.txt", "data/2-183.txt", "data/2-184-plain.txt", "data/2-184.txt", "data/2-185-plain.txt", "data/2-185.txt", "data/2-186-plain.txt", "data/2-186.txt", "data/2-187-plain.txt", "data/2-187.txt", "data/2-188-plain.txt", "data/2-188.txt", "data/2-189-plain.txt", "data/2-189.txt", "data/2-190-plain.txt", "data/2-190.txt", "data/2-191-plain.txt", "data/2-191.txt", "data/2-192-plain.txt", "data/2-192.txt", "data/2-193-plain.txt", "data/2-193.txt", "data/2-194-plain.txt", "data/2-194.txt", "data/2-195-plain.txt", "data/2-195.txt", "data/2-196-plain.txt", "data/2-196.txt", "data/2-197-plain.txt", "data/2-197.txt", "data/2-198-plain.txt", "data/2-198.txt", "data/2-199-plain.txt", "data/2-199.txt", "data/2-200-plain.txt", "data/2-200.txt", "data/2-201-plain.txt", "data/2-201.txt", "data/2-203-plain.txt", "data/2-203.txt", "data/2-204-plain.txt", "data/2-204.txt", "data/2-205-plain.txt", "data/2-205.txt", "data/2-206-plain.txt", "data/2-206.txt", "data/2-207-plain.txt", "data/2-207.txt", "data/2-208-plain.txt", "data/2-208.txt", "data/2-209-plain.txt", "data/2-209.txt", "data/2-210-plain.txt", "data/2-210.txt", "data/2-211-plain.txt", "data/2-211.txt", "data/2-212-plain.txt", "data/2-212.txt", "data/2-213-plain.txt", "data/2-213.txt", "data/2-214-plain.txt", "data/2-214.txt", "data/2-215-plain.txt", "data/2-215.txt", "data/2-216-plain.txt", "data/2-216.txt", "data/2-217-plain.txt", "data/2-217.txt", "data/2-218-plain.txt", "data/2-218.txt", "data/2-219-plain.txt", "data/2-219.txt", "data/2-220-plain.txt", "data/2-220.txt", "data/2-221-plain.txt", "data/2-221.txt", "data/2-222-plain.txt", "data/2-222.txt", "data/2-223-plain.txt", "data/2-223.txt", "data/2-224-plain.txt", "data/2-224.txt", "data/2-225-plain.txt", "data/2-225.txt", "data/2-226-plain.txt", "data/2-226.txt", "data/2-227-plain.txt", "data/2-227.txt", "data/2-228-plain.txt", "data/2-228.txt", "data/2-229-plain.txt", "data/2-229.txt", "data/2-230-plain.txt", "data/2-230.txt", "data/2-231-plain.txt", "data/2-231.txt", "data/2-232-plain.txt", "data/2-232.txt", "data/2-233-plain.txt", "data/2-233.txt", "data/2-234-plain.txt", "data/2-234.txt", "data/2-235-plain.txt", "data/2-235.txt", "data/2-236-plain.txt", "data/2-236.txt", "data/2-237-plain.txt", "data/2-237.txt", "data/2-238-plain.txt", "data/2-238.txt", "data/2-239-plain.txt", "data/2-239.txt", "data/2-240-plain.txt", "data/2-240.txt", "data/2-241-plain.txt", "data/2-241.txt", "data/2-242-plain.txt", "data/2-242.txt", "data/2-243-plain.txt", "data/2-243.txt", "data/2-244-plain.txt", "data/2-244.txt", "data/2-245-plain.txt", "data/2-245.txt", "data/2-246-plain.txt", "data/2-246.txt", "data/2-247-plain.txt", "data/2-247.txt", "data/2-248-plain.txt", "data/2-248.txt", "data/2-249-plain.txt", "data/2-249.txt", "data/2-250-plain.txt", "data/2-250.txt", "data/2-251-plain.txt", "data/2-251.txt", "data/2-252-plain.txt", "data/2-252.txt", "data/2-253-plain.txt", "data/2-253.txt", "data/2-254-plain.txt", "data/2-254.txt", "data/2-255-plain.txt", "data/2-255.txt", "data/2-256-plain.txt", "data/2-256.txt", "data/2-257-plain.txt", "data/2-257.txt", "data/2-258-plain.txt", "data/2-258.txt", "data/2-259-plain.txt", "data/2-259.txt", "data/2-260-plain.txt", "data/2-260.txt", "data/2-261-plain.txt", "data/2-261.txt", "data/2-262-plain.txt", "data/2-262.txt", "data/2-263-plain.txt", "data/2-263.txt", "data/2-264-plain.txt", "data/2-264.txt", "data/2-265-plain.txt", "data/2-265.txt", "data/2-266-plain.txt", "data/2-266.txt", "data/2-267-plain.txt", "data/2-267.txt", "data/2-268-plain.txt", "data/2-268.txt", "data/2-269-plain.txt", "data/2-269.txt", "data/2-270-plain.txt", "data/2-270.txt", "data/2-271-plain.txt", "data/2-271.txt", "data/2-272-plain.txt", "data/2-272.txt", "data/2-273-plain.txt", "data/2-273.txt", "data/2-274-plain.txt", "data/2-274.txt", "data/2-275-plain.txt", "data/2-275.txt", "data/2-276-plain.txt", "data/2-276.txt", "data/2-277-plain.txt", "data/2-277.txt", "data/2-278-plain.txt", "data/2-278.txt", "data/2-279-plain.txt", "data/2-279.txt", "data/2-280-plain.txt", "data/2-280.txt", "data/2-281-plain.txt", "data/2-281.txt", "data/2-282-plain.txt", "data/2-282.txt", "data/2-283-plain.txt", "data/2-283.txt", "data/2-284-plain.txt", "data/2-284.txt", "data/2-285-plain.txt", "data/2-285.txt", "data/2-286-plain.txt", "data/2-286.txt", "data/2-287-plain.txt", "data/2-287.txt", "data/2-288-plain.txt", "data/2-288.txt", "data/2-289-plain.txt", "data/2-289.txt", "data/2-290-plain.txt", "data/2-290.txt", "data/2-291-plain.txt", "data/2-291.txt", "data/2-292-plain.txt", "data/2-292.txt", "data/2-293-plain.txt", "data/2-293.txt", "data/2-294-plain.txt", "data/2-294.txt", "data/2-295-plain.txt", "data/2-295.txt", "data/2-296-plain.txt", "data/2-296.txt", "data/2-297-plain.txt", "data/2-297.txt", "data/2-298-plain.txt", "data/2-298.txt", "data/2-299-plain.txt", "data/2-299.txt", "data/2-300-plain.txt", "data/2-300.txt", "data/2-301-plain.txt", "data/2-301.txt", "data/2-302-plain.txt", "data/2-302.txt", "data/2-303-plain.txt", "data/2-303.txt", "data/2-304-plain.txt", "data/2-304.txt", "data/2-305-plain.txt", "data/2-305.txt", "data/2-306-plain.txt", "data/2-306.txt", "data/2-307-plain.txt", "data/2-307.txt", "data/2-308-plain.txt", "data/2-308.txt", "data/2-309-plain.txt", "data/2-309.txt", "data/2-310-plain.txt", "data/2-310.txt", "data/2-311-plain.txt", "data/2-311.txt", "data/2-312-plain.txt", "data/2-312.txt", "data/2-313-plain.txt", "data/2-313.txt", "data/2-314-plain.txt", "data/2-314.txt", "data/2-315-plain.txt", "data/2-315.txt", "data/2-316-plain.txt", "data/2-316.txt", "data/2-317-plain.txt", "data/2-317.txt", "data/2-318-plain.txt", "data/2-318.txt", "data/2-319-plain.txt", "data/2-319.txt", "data/2-320-plain.txt", "data/2-320.txt", "data/2-321-plain.txt", "data/2-321.txt", "data/2-322-plain.txt", "data/2-322.txt", "data/2-323-plain.txt", "data/2-323.txt", "data/2-324-plain.txt", "data/2-324.txt", "data/2-325-plain.txt", "data/2-325.txt", "data/2-326-plain.txt", "data/2-326.txt", "data/2-327-plain.txt", "data/2-327.txt", "data/2-328-plain.txt", "data/2-328.txt", "data/2-329-plain.txt", "data/2-329.txt", "data/2-330-plain.txt", "data/2-330.txt", "data/2-331-plain.txt", "data/2-331.txt", "data/2-332-plain.txt", "data/2-332.txt", "data/2-333-plain.txt", "data/2-333.txt", "data/2-334-plain.txt", "data/2-334.txt", "data/2-335-plain.txt", "data/2-335.txt", "data/2-336-plain.txt", "data/2-336.txt", "data/2-337-plain.txt", "data/2-337.txt", "data/2-338-plain.txt", "data/2-338.txt", "data/2-339-plain.txt", "data/2-339.txt", "data/2-340-plain.txt", "data/2-340.txt", "data/2-341-plain.txt", "data/2-341.txt", "data/2-342-plain.txt", "data/2-342.txt", "data/2-343-plain.txt", "data/2-343.txt", "data/2-344-plain.txt", "data/2-344.txt", "data/2-345-plain.txt", "data/2-345.txt", "data/2-346-plain.txt", "data/2-346.txt", "data/2-347-plain.txt", "data/2-347.txt", "data/2-348-plain.txt", "data/2-348.txt", "data/2-349-plain.txt", "data/2-349.txt", "data/2-350-plain.txt", "data/2-350.txt", "data/2-351-plain.txt", "data/2-351.txt", "data/2-352-plain.txt", "data/2-352.txt", "data/2-353-plain.txt", "data/2-353.txt", "data/2-354-plain.txt", "data/2-354.txt", "data/2-355-plain.txt", "data/2-355.txt", "data/2-356-plain.txt", "data/2-356.txt", "data/2-357-plain.txt", "data/2-357.txt", "data/2-358-plain.txt", "data/2-358.txt", "data/2-359-plain.txt", "data/2-359.txt", "data/2-360-plain.txt", "data/2-360.txt", "data/2-361-plain.txt", "data/2-361.txt", "data/2-362-plain.txt", "data/2-362.txt", "data/2-363-plain.txt", "data/2-363.txt", "data/2-364-plain.txt", "data/2-364.txt", "data/2-365-plain.txt", "data/2-365.txt", "data/2-366-plain.txt", "data/2-366.txt", "data/2-367-plain.txt", "data/2-367.txt", "data/3-001-plain.txt", "data/3-001.txt", "data/3-002-plain.txt", "data/3-002.txt", "data/3-003-plain.txt", "data/3-003.txt", "data/3-004-plain.txt", "data/3-004.txt", "data/3-005-plain.txt", "data/3-005.txt", "data/3-006-plain.txt", "data/3-006.txt", "data/3-007-plain.txt", "data/3-007.txt", "data/3-008-plain.txt", "data/3-008.txt", "data/3-009-plain.txt", "data/3-009.txt", "data/3-010-plain.txt", "data/3-010.txt", "data/3-011-plain.txt", "data/3-011.txt", "data/3-012-plain.txt", "data/3-012.txt", "data/3-013-plain.txt", "data/3-013.txt", "data/3-014-plain.txt", "data/3-014.txt", "data/3-015-plain.txt", "data/3-015.txt", "data/3-016-plain.txt", "data/3-016.txt", "data/3-017-plain.txt", "data/3-017.txt", "data/3-018-plain.txt", "data/3-018.txt", "data/3-019-plain.txt", "data/3-019.txt", "data/3-020-plain.txt", "data/3-020.txt", "data/3-021-plain.txt", "data/3-021.txt", "data/3-022-plain.txt", "data/3-022.txt", "data/3-023-plain.txt", "data/3-023.txt", "data/3-024-plain.txt", "data/3-024.txt", "data/3-025-plain.txt", "data/3-025.txt", "data/3-026-plain.txt", "data/3-026.txt", "data/3-027-plain.txt", "data/3-027.txt", "data/3-028-plain.txt", "data/3-028.txt", "data/3-029-plain.txt", "data/3-029.txt", "data/3-030-plain.txt", "data/3-030.txt", "data/3-031-plain.txt", "data/3-031.txt", "data/3-032-plain.txt", "data/3-032.txt", "data/3-033-plain.txt", "data/3-033.txt", "data/3-034-plain.txt", "data/3-034.txt", "data/3-035-plain.txt", "data/3-035.txt", "data/3-036-plain.txt", "data/3-036.txt", "data/3-037-plain.txt", "data/3-037.txt", "data/3-038-plain.txt", "data/3-038.txt", "data/3-039-plain.txt", "data/3-039.txt", "data/3-040-plain.txt", "data/3-040.txt", "data/3-041-plain.txt", "data/3-041.txt", "data/3-042-plain.txt", "data/3-042.txt", "data/3-043-plain.txt", "data/3-043.txt", "data/3-044-plain.txt", "data/3-044.txt", "data/3-045-plain.txt", "data/3-045.txt", "data/3-046-plain.txt", "data/3-046.txt", "data/3-047-plain.txt", "data/3-047.txt", "data/3-048-plain.txt", "data/3-048.txt", "data/3-049-plain.txt", "data/3-049.txt", "data/3-050-plain.txt", "data/3-050.txt", "data/3-051-plain.txt", "data/3-051.txt", "data/3-052-plain.txt", "data/3-052.txt", "data/3-053-plain.txt", "data/3-053.txt", "data/3-054-plain.txt", "data/3-054.txt", "data/3-055-plain.txt", "data/3-055.txt", "data/3-056-plain.txt", "data/3-056.txt", "data/3-057-plain.txt", "data/3-057.txt", "data/3-058-plain.txt", "data/3-058.txt", "data/3-059-plain.txt", "data/3-059.txt", "data/3-060-plain.txt", "data/3-060.txt", "data/3-061-plain.txt", "data/3-061.txt", "data/3-062-plain.txt", "data/3-062.txt", "data/3-063-plain.txt", "data/3-063.txt", "data/3-064-plain.txt", "data/3-064.txt", "data/3-065-plain.txt", "data/3-065.txt", "data/3-066-plain.txt", "data/3-066.txt", "data/3-067-plain.txt", "data/3-067.txt", "data/3-068-plain.txt", "data/3-068.txt", "data/3-069-plain.txt", "data/3-069.txt", "data/3-070-plain.txt", "data/3-070.txt", "data/3-071-plain.txt", "data/3-071.txt", "data/3-072-plain.txt", "data/3-072.txt", "data/3-073-plain.txt", "data/3-073.txt", "data/3-074-plain.txt", "data/3-074.txt", "data/3-075-plain.txt", "data/3-075.txt", "data/3-076-plain.txt", "data/3-076.txt", "data/3-077-plain.txt", "data/3-077.txt", "data/3-078-plain.txt", "data/3-078.txt", "data/3-079-plain.txt", "data/3-079.txt", "data/3-080-plain.txt", "data/3-080.txt", "data/3-081-plain.txt", "data/3-081.txt", "data/3-082-plain.txt", "data/3-082.txt", "data/3-083-plain.txt", "data/3-083.txt", "data/3-084-plain.txt", "data/3-084.txt", "data/3-085-plain.txt", "data/3-085.txt", "data/3-086-plain.txt", "data/3-086.txt", "data/3-087-plain.txt", "data/3-087.txt", "data/3-088-plain.txt", "data/3-088.txt", "data/3-089-plain.txt", "data/3-089.txt", "data/3-090-plain.txt", "data/3-090.txt", "data/3-091-plain.txt", "data/3-091.txt", "data/3-092-plain.txt", "data/3-092.txt", "data/3-093-plain.txt", "data/3-093.txt", "data/3-094-plain.txt", "data/3-094.txt", "data/3-095-plain.txt", "data/3-095.txt", "data/3-096-plain.txt", "data/3-096.txt", "data/3-097-plain.txt", "data/3-097.txt", "data/3-098-plain.txt", "data/3-098.txt", "data/3-099-plain.txt", "data/3-099.txt", "data/3-100-plain.txt", "data/3-100.txt", "data/3-101-plain.txt", "data/3-101.txt", "data/3-103-plain.txt", "data/3-103.txt", "data/3-104-plain.txt", "data/3-104.txt", "data/3-105-plain.txt", "data/3-105.txt", "data/3-106-plain.txt", "data/3-106.txt", "data/3-107-plain.txt", "data/3-107.txt", "data/3-108-plain.txt", "data/3-108.txt", "data/3-109-plain.txt", "data/3-109.txt", "data/3-110-plain.txt", "data/3-110.txt", "data/3-111-plain.txt", "data/3-111.txt", "data/3-112-plain.txt", "data/3-112.txt", "data/3-113-plain.txt", "data/3-113.txt", "data/3-114-plain.txt", "data/3-114.txt", "data/3-115-plain.txt", "data/3-115.txt", "data/3-119-plain.txt", "data/3-119.txt", "data/3-120-plain.txt", "data/3-120.txt", "data/3-121-plain.txt", "data/3-121.txt", "data/3-122-plain.txt", "data/3-122.txt", "data/3-123-plain.txt", "data/3-123.txt", "data/3-124-plain.txt", "data/3-124.txt", "data/3-125-plain.txt", "data/3-125.txt", "data/3-126-plain.txt", "data/3-126.txt", "data/3-127-plain.txt", "data/3-127.txt", "data/3-128-plain.txt", "data/3-128.txt", "data/3-129-plain.txt", "data/3-129.txt", "data/3-130-plain.txt", "data/3-130.txt", "data/3-131-plain.txt", "data/3-131.txt", "data/3-132-plain.txt", "data/3-132.txt", "data/3-133-plain.txt", "data/3-133.txt", "data/3-134-plain.txt", "data/3-134.txt", "data/3-135-plain.txt", "data/3-135.txt", "data/3-136-plain.txt", "data/3-136.txt", "data/3-137-plain.txt", "data/3-137.txt", "data/3-138-plain.txt", "data/3-138.txt", "data/3-139-plain.txt", "data/3-139.txt", "data/3-140-plain.txt", "data/3-140.txt", "data/3-141-plain.txt", "data/3-141.txt", "data/3-142-plain.txt", "data/3-142.txt", "data/3-143-plain.txt", "data/3-143.txt", "data/3-144-plain.txt", "data/3-144.txt", "data/3-145-plain.txt", "data/3-145.txt", "data/3-146-plain.txt", "data/3-146.txt", "data/3-147-plain.txt", "data/3-147.txt", "data/3-148-plain.txt", "data/3-148.txt", "data/3-149-plain.txt", "data/3-149.txt", "data/3-150-plain.txt", "data/3-150.txt", "data/3-151-plain.txt", "data/3-151.txt", "data/3-152-plain.txt", "data/3-152.txt", "data/3-153-plain.txt", "data/3-153.txt", "data/3-154-plain.txt", "data/3-154.txt", "data/3-155-plain.txt", "data/3-155.txt", "data/</t>
   </si>
   <si>
@@ -139,7 +136,7 @@
     <t>COOEE_contents.xlsx</t>
   </si>
   <si>
-    <t>2021-11-10T14:57:05+11:00</t>
+    <t>2021-11-13T12:10:41+11:00</t>
   </si>
   <si>
     <t>["https://www.nationalarchives.gov.uk/PRONOM/fmt/214", application/vnd.openxmlformats-officedocument.spreadsheetml.sheet]</t>
@@ -711,13 +708,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="5" width="20" customWidth="1"/>
+    <col min="1" max="4" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -725,16 +722,13 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -746,9 +740,6 @@
       </c>
       <c r="D2" t="s">
         <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -773,16 +764,16 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
         <v>26</v>
-      </c>
-      <c r="D1" t="s">
-        <v>27</v>
       </c>
       <c r="E1" t="s">
         <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G1" t="s">
         <v>16</v>
@@ -790,22 +781,22 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
         <v>29</v>
-      </c>
-      <c r="B2" t="s">
-        <v>30</v>
       </c>
       <c r="C2">
         <v>113152</v>
       </c>
       <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
         <v>31</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>32</v>
-      </c>
-      <c r="F2" t="s">
-        <v>33</v>
       </c>
       <c r="G2" t="s">
         <v>17</v>
@@ -813,94 +804,88 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3">
         <v>544768</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" t="s">
         <v>35</v>
       </c>
-      <c r="F3" t="s">
-        <v>36</v>
-      </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4">
         <v>1789440</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" t="s">
         <v>36</v>
-      </c>
-      <c r="G4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5">
+        <v>190263</v>
+      </c>
+      <c r="D5" t="s">
         <v>39</v>
       </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5">
-        <v>190259</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>40</v>
       </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" t="s">
-        <v>41</v>
-      </c>
       <c r="G5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6">
         <v>190095</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="F6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" t="s">
         <v>41</v>
-      </c>
-      <c r="G6" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -930,13 +915,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
         <v>44</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>45</v>
-      </c>
-      <c r="C2" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -961,30 +946,30 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
         <v>49</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>50</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>51</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>52</v>
-      </c>
-      <c r="E2" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1014,46 +999,46 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
         <v>54</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>55</v>
-      </c>
-      <c r="C2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
         <v>57</v>
-      </c>
-      <c r="B3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
         <v>59</v>
-      </c>
-      <c r="B4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>